<commit_message>
Move J1 to bottom layer Add J1 to J3 connectors to BOM for quotes
</commit_message>
<xml_diff>
--- a/BOM - WIFI RELAY NODE.xlsx
+++ b/BOM - WIFI RELAY NODE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\David\PROJECTS\EAGLE\Wifi Relay Node\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE68DBC-D66D-4B51-917D-5AF4AF4C18B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E57926F-F590-4D36-A197-0BFC2E0C0D7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="276" windowWidth="20376" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2-ESP-wroom-02U" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="115">
   <si>
     <t>Qty</t>
   </si>
@@ -100,9 +100,6 @@
     <t>Espressif Systems</t>
   </si>
   <si>
-    <t>1X02</t>
-  </si>
-  <si>
     <t>J2</t>
   </si>
   <si>
@@ -112,15 +109,9 @@
     <t>MICROCHIP</t>
   </si>
   <si>
-    <t>1X06</t>
-  </si>
-  <si>
     <t>J3</t>
   </si>
   <si>
-    <t>2X10</t>
-  </si>
-  <si>
     <t>J4</t>
   </si>
   <si>
@@ -319,16 +310,61 @@
     <t>8-pin male header</t>
   </si>
   <si>
-    <t>16-pin Female header</t>
-  </si>
-  <si>
-    <t>6-Pin Male</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
     <t>U3</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/sullins-connector-solutions/PPTC102LFBN-RC/S7078-ND/810216</t>
+  </si>
+  <si>
+    <t>S7078-ND</t>
+  </si>
+  <si>
+    <t>20-pin Female header</t>
+  </si>
+  <si>
+    <t>PPTC102LFBN-RC</t>
+  </si>
+  <si>
+    <t>Sullins</t>
+  </si>
+  <si>
+    <t>952-2262-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/harwin-inc/M20-9990246/952-2262-ND/3728226</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Harwin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> M20-9990246</t>
+  </si>
+  <si>
+    <t>1X02 (Pitch 2.54mm)</t>
+  </si>
+  <si>
+    <t>1X06 (Pitch 2.54mm)</t>
+  </si>
+  <si>
+    <t>2X10 (Pitch 2.54mm)</t>
+  </si>
+  <si>
+    <t>609-3263-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/amphenol-icc-fci/68000-406HLF/609-3263-ND/1878471</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Amphenol</t>
+  </si>
+  <si>
+    <t>68000-406HLF</t>
+  </si>
+  <si>
+    <t>6-Pin male header</t>
   </si>
 </sst>
 </file>
@@ -1231,7 +1267,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1289,10 +1325,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>11</v>
@@ -1301,19 +1337,19 @@
         <v>12</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K2" s="15">
         <v>0.34</v>
@@ -1327,28 +1363,28 @@
         <v>13</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K3" s="15">
         <v>0.1</v>
@@ -1362,28 +1398,28 @@
         <v>18</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K4" s="15">
         <v>0.37</v>
@@ -1400,25 +1436,25 @@
         <v>16</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G5" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>70</v>
       </c>
       <c r="K5" s="15">
         <v>0.1</v>
@@ -1441,19 +1477,19 @@
         <v>22</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K6" s="15">
         <v>0.1</v>
@@ -1464,19 +1500,19 @@
         <v>1</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K7" s="15"/>
     </row>
@@ -1491,19 +1527,19 @@
         <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>25</v>
@@ -1520,94 +1556,136 @@
         <v>1</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D9" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>27</v>
-      </c>
       <c r="F9" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="K9" s="15"/>
+        <v>94</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="K9" s="15">
+        <v>0.11</v>
+      </c>
     </row>
     <row r="10" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>1</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="K10" s="15"/>
+        <v>114</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="K10" s="15">
+        <v>0.27</v>
+      </c>
     </row>
     <row r="11" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>1</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="12" t="s">
+      <c r="H11" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11" s="15"/>
+      <c r="K11" s="15">
+        <v>1.3</v>
+      </c>
     </row>
     <row r="12" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>1</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K12" s="15">
         <v>0.39</v>
@@ -1618,31 +1696,31 @@
         <v>1</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C13" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="E13" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>93</v>
-      </c>
       <c r="J13" s="17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K13" s="19">
         <v>1.66</v>
@@ -1653,31 +1731,31 @@
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="I14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="K14" s="5">
         <v>1.51</v>
@@ -1688,31 +1766,31 @@
         <v>1</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="J15" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K15" s="11">
         <v>1.2</v>
@@ -1731,8 +1809,11 @@
     <hyperlink ref="H13" r:id="rId8" xr:uid="{6B0C927C-8C67-40A0-A59F-AAE21B75B073}"/>
     <hyperlink ref="H14" r:id="rId9" xr:uid="{3E23A451-8DBF-47A2-BF54-D403D8F1F106}"/>
     <hyperlink ref="H15" r:id="rId10" xr:uid="{4100F47A-0306-4166-A547-EFA692A083A8}"/>
+    <hyperlink ref="H11" r:id="rId11" xr:uid="{19C7F617-3DFB-4832-A6A1-32BADDFF236F}"/>
+    <hyperlink ref="H9" r:id="rId12" xr:uid="{9D53D35F-6756-45EC-A666-78EC673350D0}"/>
+    <hyperlink ref="H10" r:id="rId13" xr:uid="{4D48A1DC-3377-47FF-B044-EFADE2FF5C9D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Replace I/O expander to MCP23018 28-SOIC Replace BOM part numbers to match JLCPB inventory
</commit_message>
<xml_diff>
--- a/BOM - WIFI RELAY NODE.xlsx
+++ b/BOM - WIFI RELAY NODE.xlsx
@@ -8,19 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\David\PROJECTS\EAGLE\Wifi Relay Node\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E57926F-F590-4D36-A197-0BFC2E0C0D7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E54317F-B501-4975-8254-326EAABF8B15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="276" windowWidth="20376" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2-ESP-wroom-02U" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="131">
   <si>
     <t>Qty</t>
   </si>
@@ -169,9 +177,6 @@
     <t>https://www.digikey.com/product-detail/en/on-semiconductor/MBR0520LT3G/MBR0520LT3GOSCT-ND/2705022</t>
   </si>
   <si>
-    <t xml:space="preserve"> MBR0520LT3GOSCT-ND</t>
-  </si>
-  <si>
     <t>ON Semiconductor</t>
   </si>
   <si>
@@ -365,6 +370,103 @@
   </si>
   <si>
     <t>6-Pin male header</t>
+  </si>
+  <si>
+    <t>Extended price</t>
+  </si>
+  <si>
+    <t>Voltage regulator 3.3 V - 500 mA</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>For JLCPCB</t>
+  </si>
+  <si>
+    <t>MIC5504-3.3</t>
+  </si>
+  <si>
+    <t>Voltage regulator 3.3 V - 300 mA</t>
+  </si>
+  <si>
+    <t>MIC5504-3.3YM5-TR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/MIC5504-3-3YM5-TR/576-4764-1-ND/4864028</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Microchip Technology</t>
+  </si>
+  <si>
+    <t>576-4764-1-ND</t>
+  </si>
+  <si>
+    <t>For JLCPCB - Digikey had 0 stock</t>
+  </si>
+  <si>
+    <t>MCP23018-E/SO</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> MBR0520</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LT1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GOSCT-ND</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> MBR0520</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LT3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GOSCT-ND</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/MCP23018-E-SO/MCP23018-E-SO-ND/1999504</t>
+  </si>
+  <si>
+    <t>MCP23018-E/SO-ND</t>
+  </si>
+  <si>
+    <t>Larger pitch to make it easier to solder by hand</t>
   </si>
 </sst>
 </file>
@@ -541,7 +643,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -719,6 +821,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -883,7 +991,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -908,6 +1016,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1264,28 +1383,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="66.5546875" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1319,16 +1440,22 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>11</v>
@@ -1337,16 +1464,16 @@
         <v>12</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>49</v>
+        <v>127</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>48</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>46</v>
@@ -1354,466 +1481,680 @@
       <c r="K2" s="15">
         <v>0.34</v>
       </c>
+      <c r="L2" s="15">
+        <f>K2*A2</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
+    <row r="3" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="23">
+        <v>0.04</v>
+      </c>
+      <c r="L3" s="23">
+        <f>K3*A3</f>
+        <v>0.08</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="13"/>
+      <c r="H4" s="14"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+    </row>
+    <row r="5" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
         <v>5</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="C5" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="14" t="s">
+      <c r="H5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="15">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
-        <v>4</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="K4" s="15">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
-        <v>4</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>66</v>
-      </c>
       <c r="J5" s="12" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="K5" s="15">
         <v>0.1</v>
       </c>
+      <c r="L5" s="15">
+        <f t="shared" ref="L5:L22" si="0">K5*A5</f>
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="15">
+        <v>0.37</v>
+      </c>
+      <c r="L6" s="15">
+        <f t="shared" si="0"/>
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <v>4</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="K7" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="L7" s="15">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12">
         <v>3</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D8" s="16">
         <v>603</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G8" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="I8" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="K6" s="15">
+      <c r="K8" s="15">
         <v>0.1</v>
       </c>
+      <c r="L8" s="15">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
-        <v>1</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="15"/>
-    </row>
-    <row r="8" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
-        <v>1</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="15">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>94</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="K9" s="15">
-        <v>0.11</v>
+        <v>35</v>
+      </c>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>1</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>114</v>
+        <v>23</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>114</v>
+        <v>36</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>110</v>
+        <v>72</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>112</v>
+        <v>25</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>113</v>
+        <v>23</v>
       </c>
       <c r="K10" s="15">
-        <v>0.27</v>
+        <v>3.2</v>
+      </c>
+      <c r="L10" s="15">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>1</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="K11" s="15">
-        <v>1.3</v>
+        <v>0.11</v>
+      </c>
+      <c r="L11" s="15">
+        <f t="shared" si="0"/>
+        <v>0.11</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>1</v>
       </c>
       <c r="B12" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="K12" s="15">
+        <v>0.27</v>
+      </c>
+      <c r="L12" s="15">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>1</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="K13" s="15">
+        <v>1.3</v>
+      </c>
+      <c r="L13" s="15">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12">
+        <v>0</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C15" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="K15" s="15">
+        <v>0.39</v>
+      </c>
+      <c r="L15" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="20">
+        <v>1</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="F12" s="12" t="s">
+      <c r="G16" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="K16" s="23">
+        <v>0.11</v>
+      </c>
+      <c r="L16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11</v>
+      </c>
+      <c r="M16" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="13"/>
+      <c r="H17" s="14"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17">
+        <v>0</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K12" s="15">
-        <v>0.39</v>
+      <c r="K18" s="19">
+        <v>1.66</v>
+      </c>
+      <c r="L18" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17">
+    <row r="19" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="24">
         <v>1</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="17" t="s">
+      <c r="B19" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="G13" s="17" t="s">
+      <c r="F19" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="G19" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="K19" s="25">
+        <v>1.51</v>
+      </c>
+      <c r="L19" s="23">
+        <f t="shared" si="0"/>
+        <v>1.51</v>
+      </c>
+      <c r="M19" s="24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="18"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="15"/>
+    </row>
+    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>0</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="D21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J13" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="K13" s="19">
-        <v>1.66</v>
+      <c r="H21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K21" s="5">
+        <v>1.51</v>
+      </c>
+      <c r="L21" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>1</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="7" t="s">
+    <row r="22" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
+        <v>0</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="C22" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="K14" s="5">
-        <v>1.51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
-        <v>1</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" s="8" t="s">
+      <c r="F22" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="K15" s="11">
+      <c r="K22" s="11">
         <v>1.2</v>
+      </c>
+      <c r="L22" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{7A16E887-5AEF-4F63-9D0E-69E24586E962}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{5AE20744-6278-48FF-826C-E165DB38D0EB}"/>
-    <hyperlink ref="H8" r:id="rId6" xr:uid="{BBEE8BD8-67D1-4A7E-ABE9-BB7896F7CFBE}"/>
-    <hyperlink ref="H12" r:id="rId7" xr:uid="{EC3314D4-DA5D-4457-AE84-5B27C92D554B}"/>
-    <hyperlink ref="H13" r:id="rId8" xr:uid="{6B0C927C-8C67-40A0-A59F-AAE21B75B073}"/>
-    <hyperlink ref="H14" r:id="rId9" xr:uid="{3E23A451-8DBF-47A2-BF54-D403D8F1F106}"/>
-    <hyperlink ref="H15" r:id="rId10" xr:uid="{4100F47A-0306-4166-A547-EFA692A083A8}"/>
-    <hyperlink ref="H11" r:id="rId11" xr:uid="{19C7F617-3DFB-4832-A6A1-32BADDFF236F}"/>
-    <hyperlink ref="H9" r:id="rId12" xr:uid="{9D53D35F-6756-45EC-A666-78EC673350D0}"/>
-    <hyperlink ref="H10" r:id="rId13" xr:uid="{4D48A1DC-3377-47FF-B044-EFADE2FF5C9D}"/>
+    <hyperlink ref="H5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H7" r:id="rId4" xr:uid="{7A16E887-5AEF-4F63-9D0E-69E24586E962}"/>
+    <hyperlink ref="H8" r:id="rId5" xr:uid="{5AE20744-6278-48FF-826C-E165DB38D0EB}"/>
+    <hyperlink ref="H10" r:id="rId6" xr:uid="{BBEE8BD8-67D1-4A7E-ABE9-BB7896F7CFBE}"/>
+    <hyperlink ref="H15" r:id="rId7" xr:uid="{EC3314D4-DA5D-4457-AE84-5B27C92D554B}"/>
+    <hyperlink ref="H18" r:id="rId8" xr:uid="{6B0C927C-8C67-40A0-A59F-AAE21B75B073}"/>
+    <hyperlink ref="H21" r:id="rId9" xr:uid="{3E23A451-8DBF-47A2-BF54-D403D8F1F106}"/>
+    <hyperlink ref="H22" r:id="rId10" xr:uid="{4100F47A-0306-4166-A547-EFA692A083A8}"/>
+    <hyperlink ref="H13" r:id="rId11" xr:uid="{19C7F617-3DFB-4832-A6A1-32BADDFF236F}"/>
+    <hyperlink ref="H11" r:id="rId12" xr:uid="{9D53D35F-6756-45EC-A666-78EC673350D0}"/>
+    <hyperlink ref="H12" r:id="rId13" xr:uid="{4D48A1DC-3377-47FF-B044-EFADE2FF5C9D}"/>
+    <hyperlink ref="H16" r:id="rId14" xr:uid="{0D8C85AC-B36A-411B-AC8F-55F76DFE721A}"/>
+    <hyperlink ref="H3" r:id="rId15" xr:uid="{753F75CE-7437-448D-84D5-9557ECD16509}"/>
+    <hyperlink ref="H19" r:id="rId16" xr:uid="{25289B2F-F195-4273-A002-F5165BF0FCFA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor changes for production PCB ordered -  v1.0.0
</commit_message>
<xml_diff>
--- a/BOM - WIFI RELAY NODE.xlsx
+++ b/BOM - WIFI RELAY NODE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\David\PROJECTS\EAGLE\Wifi Relay Node\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E54317F-B501-4975-8254-326EAABF8B15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83DD9CC-F3CF-4906-84FA-B324FEB7A74D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="276" windowWidth="20376" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2-ESP-wroom-02U" sheetId="1" r:id="rId1"/>
@@ -1386,7 +1386,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>